<commit_message>
close contract from January to March
</commit_message>
<xml_diff>
--- a/29.04-17.05.xlsx
+++ b/29.04-17.05.xlsx
@@ -74,6 +74,30 @@
           </rPr>
           <t xml:space="preserve">
 с учетом сокращенного дня переработка полтора часа. В сумме остается недоработка 2 часа</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M22" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Anna Sharuntsova.EXT:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+по контракту работаю до 15.05, т.е. 15 часов на этой неделе, плюс 2 часа переработки за долги</t>
         </r>
       </text>
     </comment>
@@ -266,19 +290,19 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -569,7 +593,7 @@
   <dimension ref="B2:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22:H23"/>
+      <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,7 +621,7 @@
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1"/>
@@ -619,7 +643,7 @@
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="9"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="1"/>
       <c r="D4" s="6"/>
       <c r="E4" s="1">
@@ -641,17 +665,17 @@
       <c r="C6" s="1">
         <v>0.67708333333333337</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>3.5</v>
       </c>
       <c r="E6" s="1">
         <v>0.63541666666666663</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="9">
         <v>2.5</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="10"/>
+      <c r="H6" s="9"/>
       <c r="I6" s="1"/>
       <c r="J6" s="8"/>
       <c r="K6" s="1"/>
@@ -665,13 +689,13 @@
       <c r="C7" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="1">
         <v>0.73958333333333337</v>
       </c>
-      <c r="F7" s="10"/>
+      <c r="F7" s="9"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="10"/>
+      <c r="H7" s="9"/>
       <c r="I7" s="1"/>
       <c r="J7" s="8"/>
       <c r="K7" s="1"/>
@@ -700,7 +724,7 @@
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="1">
@@ -718,7 +742,7 @@
       <c r="G11" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="13">
         <v>6</v>
       </c>
       <c r="I11" s="1"/>
@@ -728,7 +752,7 @@
       <c r="M11" s="7"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="9"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="1">
         <v>0.8125</v>
       </c>
@@ -740,7 +764,7 @@
       <c r="G12" s="1">
         <v>0.83333333333333337</v>
       </c>
-      <c r="H12" s="11"/>
+      <c r="H12" s="13"/>
       <c r="I12" s="1"/>
       <c r="J12" s="6"/>
       <c r="K12" s="1"/>
@@ -754,13 +778,13 @@
       <c r="C14" s="1">
         <v>0.52083333333333337</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <v>6</v>
       </c>
       <c r="E14" s="1">
         <v>0.63541666666666663</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="9">
         <v>3.5</v>
       </c>
       <c r="G14" s="1">
@@ -782,11 +806,11 @@
       <c r="C15" s="1">
         <v>0.8125</v>
       </c>
-      <c r="D15" s="10"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="1">
         <v>0.78125</v>
       </c>
-      <c r="F15" s="10"/>
+      <c r="F15" s="9"/>
       <c r="G15" s="1">
         <v>0.83333333333333337</v>
       </c>
@@ -819,7 +843,7 @@
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="1"/>
@@ -835,7 +859,7 @@
       <c r="M19" s="7"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="9"/>
+      <c r="B20" s="10"/>
       <c r="C20" s="1"/>
       <c r="D20" s="6"/>
       <c r="E20" s="1"/>
@@ -870,11 +894,17 @@
       <c r="H22" s="8">
         <v>4</v>
       </c>
-      <c r="I22" s="1"/>
-      <c r="J22" s="8"/>
+      <c r="I22" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="J22" s="8">
+        <v>2</v>
+      </c>
       <c r="K22" s="5"/>
       <c r="L22" s="8"/>
-      <c r="M22" s="7"/>
+      <c r="M22" s="7">
+        <v>17</v>
+      </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
@@ -890,7 +920,9 @@
         <v>0.76041666666666663</v>
       </c>
       <c r="H23" s="8"/>
-      <c r="I23" s="1"/>
+      <c r="I23" s="1">
+        <v>0.78125</v>
+      </c>
       <c r="J23" s="8"/>
       <c r="K23" s="1"/>
       <c r="L23" s="8"/>
@@ -912,15 +944,15 @@
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="6"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="12"/>
+      <c r="F27" s="11"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="12"/>
+      <c r="H27" s="11"/>
       <c r="I27" s="1"/>
       <c r="J27" s="6"/>
       <c r="K27" s="1"/>
@@ -928,13 +960,13 @@
       <c r="M27" s="7"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="9"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="1"/>
       <c r="D28" s="6"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="13"/>
+      <c r="F28" s="12"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="13"/>
+      <c r="H28" s="12"/>
       <c r="I28" s="1"/>
       <c r="J28" s="6"/>
       <c r="K28" s="1"/>
@@ -946,33 +978,75 @@
         <v>2</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="10"/>
+      <c r="D30" s="9"/>
       <c r="E30" s="1"/>
       <c r="F30" s="8"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="10"/>
+      <c r="H30" s="9"/>
       <c r="I30" s="1"/>
       <c r="J30" s="8"/>
       <c r="K30" s="1"/>
-      <c r="L30" s="10"/>
+      <c r="L30" s="9"/>
       <c r="M30" s="7"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="8"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="10"/>
+      <c r="D31" s="9"/>
       <c r="E31" s="1"/>
       <c r="F31" s="8"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="10"/>
+      <c r="H31" s="9"/>
       <c r="I31" s="1"/>
       <c r="J31" s="8"/>
       <c r="K31" s="1"/>
-      <c r="L31" s="10"/>
+      <c r="L31" s="9"/>
       <c r="M31" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="J11:J12"/>
     <mergeCell ref="J27:J28"/>
     <mergeCell ref="L27:L28"/>
     <mergeCell ref="M27:M28"/>
@@ -987,48 +1061,6 @@
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="F27:F28"/>
     <mergeCell ref="H27:H28"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="J19:J20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>